<commit_message>
Data connectors completely done
</commit_message>
<xml_diff>
--- a/src/test/resources/Testsuite.xlsx
+++ b/src/test/resources/Testsuite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Create Datasets from connectors</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +460,20 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to the Create Datesets for Assertion
</commit_message>
<xml_diff>
--- a/src/test/resources/Testsuite.xlsx
+++ b/src/test/resources/Testsuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="22800" windowHeight="3885"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15840" windowHeight="4440"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -406,7 +407,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +456,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,7 +512,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>